<commit_message>
update ganti data terbaru
</commit_message>
<xml_diff>
--- a/sprint_projects.xlsx
+++ b/sprint_projects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Full Kuliah\Semester 7\Pembelajaran Mesin\Praktikum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Full Kuliah\Semester 7\Pembelajaran Mesin\Praktikum\Kelompok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5052982-E201-443D-BDB6-41472F6AC427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E357C9D3-FC7D-48AF-823E-185FFA4CD9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{1513089F-A891-47A2-BFE0-5EC6A9050994}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Task</t>
   </si>
@@ -55,12 +55,36 @@
   </si>
   <si>
     <t>Selesai</t>
+  </si>
+  <si>
+    <t>Preprocessing data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 Oktober 2021 </t>
+  </si>
+  <si>
+    <t>25 Oktober 2021</t>
+  </si>
+  <si>
+    <t>Bibit</t>
+  </si>
+  <si>
+    <t>Pemilihan Model (Modelling, Model Interface)</t>
+  </si>
+  <si>
+    <t>31 Oktober 2021</t>
+  </si>
+  <si>
+    <t>Dharma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,10 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,16 +454,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{207F3C0C-A1C9-42DB-A38C-8425CC8A4401}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -483,6 +509,46 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44509</v>
+      </c>
+      <c r="D4" s="3">
+        <v>44507</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>